<commit_message>
Import / Export XL #25 - progress
</commit_message>
<xml_diff>
--- a/test/go/tests/bckp-xl/bckp.xlsx
+++ b/test/go/tests/bckp-xl/bckp.xlsx
@@ -18,12 +18,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>Japan</t>
+  </si>
   <si>
     <t>A1</t>
   </si>
   <si>
+    <t>ENUM_VAL1_NOT_THE_SAME</t>
+  </si>
+  <si>
+    <t>1h3m0.001s</t>
+  </si>
+  <si>
     <t>A2</t>
+  </si>
+  <si>
+    <t>0s</t>
   </si>
   <si>
     <t>B1</t>
@@ -66,8 +84,11 @@
       <alignment horizontal="general" indent="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf applyAlignment="0" applyBorder="0" applyFont="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFont="0" applyFill="0" applyNumberFormat="1" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="22">
       <alignment horizontal="general" indent="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
@@ -399,7 +420,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -411,70 +432,87 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="b">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v/>
-      </c>
-      <c r="D1" t="s">
-        <v/>
-      </c>
-      <c r="E1" t="s">
-        <v/>
-      </c>
-      <c r="F1" t="s">
-        <v/>
-      </c>
-      <c r="G1">
-        <v>0</v>
-      </c>
-      <c r="H1">
-        <v>10.2</v>
-      </c>
-      <c r="I1">
-        <v>0</v>
-      </c>
-      <c r="J1" t="b">
-        <v>1</v>
-      </c>
-      <c r="K1">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1">
+        <v>44247.84171296297</v>
+      </c>
+      <c r="C2" t="b">
         <v>1</v>
       </c>
-      <c r="B2" t="b">
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v/>
+      </c>
+      <c r="F2" t="s">
+        <v/>
+      </c>
+      <c r="G2" t="s">
+        <v/>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>10.2</v>
+      </c>
+      <c r="J2">
+        <v>4</v>
+      </c>
+      <c r="K2" t="b">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
-        <v/>
-      </c>
-      <c r="D2" t="s">
-        <v/>
-      </c>
-      <c r="E2" t="s">
-        <v/>
-      </c>
-      <c r="F2" t="s">
-        <v/>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
+      <c r="L2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1">
+        <v>-693593</v>
+      </c>
+      <c r="C3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v/>
+      </c>
+      <c r="E3" t="s">
+        <v/>
+      </c>
+      <c r="F3" t="s">
+        <v/>
+      </c>
+      <c r="G3" t="s">
+        <v/>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
         <v>10.77</v>
       </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2" t="b">
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3" t="b">
         <v>1</v>
       </c>
-      <c r="K2">
-        <v>0</v>
+      <c r="L3" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -496,7 +534,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B1">
         <v>0</v>
@@ -507,7 +545,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B2">
         <v>0</v>

</xml_diff>

<commit_message>
Import / Export XL #25 - export basic fields
</commit_message>
<xml_diff>
--- a/test/go/tests/bckp-xl/bckp.xlsx
+++ b/test/go/tests/bckp-xl/bckp.xlsx
@@ -18,15 +18,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>India</t>
-  </si>
-  <si>
-    <t>Canada</t>
-  </si>
-  <si>
-    <t>Japan</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Booleanfield</t>
+  </si>
+  <si>
+    <t>Aenum</t>
+  </si>
+  <si>
+    <t>Aenum_2</t>
+  </si>
+  <si>
+    <t>Benum</t>
+  </si>
+  <si>
+    <t>CName</t>
+  </si>
+  <si>
+    <t>CFloatfield</t>
+  </si>
+  <si>
+    <t>Floatfield</t>
+  </si>
+  <si>
+    <t>Intfield</t>
+  </si>
+  <si>
+    <t>Anotherbooleanfield</t>
+  </si>
+  <si>
+    <t>Duration1</t>
   </si>
   <si>
     <t>A1</t>
@@ -438,10 +465,37 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1">
         <v>44247.84171296297</v>
@@ -450,7 +504,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="E2" t="s">
         <v/>
@@ -474,12 +528,12 @@
         <v>1</v>
       </c>
       <c r="L2" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1">
         <v>-693593</v>
@@ -512,7 +566,7 @@
         <v>1</v>
       </c>
       <c r="L3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -524,7 +578,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -534,23 +588,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>8</v>
       </c>
-      <c r="B1">
-        <v>0</v>
-      </c>
-      <c r="C1">
-        <v>0</v>
+      <c r="C1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
         <v>0</v>
       </c>
     </row>
@@ -570,6 +635,12 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Import / Export XL Fixes #25
</commit_message>
<xml_diff>
--- a/test/go/tests/bckp-xl/bckp.xlsx
+++ b/test/go/tests/bckp-xl/bckp.xlsx
@@ -18,7 +18,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+  <si>
+    <t>ID</t>
+  </si>
   <si>
     <t>Name</t>
   </si>
@@ -447,7 +450,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -492,22 +495,25 @@
       <c r="L1" t="s">
         <v>11</v>
       </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="1">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1">
         <v>44247.84171296297</v>
       </c>
-      <c r="C2" t="b">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
+      <c r="D2" t="b">
+        <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v/>
+        <v>14</v>
       </c>
       <c r="F2" t="s">
         <v/>
@@ -515,34 +521,37 @@
       <c r="G2" t="s">
         <v/>
       </c>
-      <c r="H2">
-        <v>0</v>
+      <c r="H2" t="s">
+        <v/>
       </c>
       <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
         <v>10.2</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>4</v>
       </c>
-      <c r="K2" t="b">
-        <v>1</v>
-      </c>
-      <c r="L2" t="s">
-        <v>14</v>
+      <c r="L2" t="b">
+        <v>1</v>
+      </c>
+      <c r="M2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="1">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="1">
         <v>-693593</v>
       </c>
-      <c r="C3" t="b">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v/>
+      <c r="D3" t="b">
+        <v>1</v>
       </c>
       <c r="E3" t="s">
         <v/>
@@ -553,20 +562,23 @@
       <c r="G3" t="s">
         <v/>
       </c>
-      <c r="H3">
-        <v>0</v>
+      <c r="H3" t="s">
+        <v/>
       </c>
       <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
         <v>10.77</v>
       </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3" t="b">
-        <v>1</v>
-      </c>
-      <c r="L3" t="s">
-        <v>16</v>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3" t="b">
+        <v>1</v>
+      </c>
+      <c r="M3" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -578,7 +590,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -591,31 +603,40 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>9</v>
       </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
       </c>
       <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
         <v>0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
       </c>
       <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
         <v>0</v>
       </c>
     </row>
@@ -628,7 +649,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -640,6 +661,9 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
 </worksheet>

</xml_diff>